<commit_message>
Added updated code and report
</commit_message>
<xml_diff>
--- a/Simulation_Results/Results_Summary.xlsx
+++ b/Simulation_Results/Results_Summary.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SEM 8\SRE\Simulation_Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8E6A32E-12DA-43D8-9C9D-81FC3388D8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A250261-25E4-43E5-9E15-F3FB921DFF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5EE13269-6EB3-4804-8369-6875984710C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{5EE13269-6EB3-4804-8369-6875984710C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Noise Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>muzzle_test_1</t>
   </si>
@@ -96,6 +97,9 @@
   </si>
   <si>
     <t>Mean Error</t>
+  </si>
+  <si>
+    <t>Noise (dbW)</t>
   </si>
 </sst>
 </file>
@@ -103,7 +107,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -136,7 +140,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,6 +156,1073 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Variation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Error with Noise</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Noise Test'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Noise Test'!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Noise Test'!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.27553571700888568</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28053571700888824</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27453571700888801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27653571700888335</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27753571700888813</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8310-4AE9-A83C-752A8AB9D898}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="770477936"/>
+        <c:axId val="770477104"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="770477936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Noise</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t> Power (dbW)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="770477104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="770477104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.31000000000000005"/>
+          <c:min val="0.25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Error in Bearing Angle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="770477936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC4BD5C7-E9C1-7A65-FBAC-D14FBD2A935A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,22 +1522,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB5E3CC-1B54-40EC-B3D0-65328E39CA27}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="2.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -486,7 +1557,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -508,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -537,7 +1608,7 @@
         <v>0.20148211155388918</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -559,7 +1630,7 @@
         <v>0.18559051364818657</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -581,7 +1652,7 @@
         <v>0.12410235415597981</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -603,7 +1674,7 @@
         <v>0.16619174590991292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -624,8 +1695,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f>SQRT(SUMSQ(F2:F15)/COUNTA(F2:F15))</f>
+        <v>0.30145937239130138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -647,7 +1722,7 @@
         <v>7.3881296942218455E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -669,7 +1744,7 @@
         <v>0.21500000000000341</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -691,7 +1766,7 @@
         <v>0.43705117707798991</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -713,7 +1788,7 @@
         <v>0.16999999999998749</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -735,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -757,7 +1832,7 @@
         <v>0.25019174590988769</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -779,7 +1854,7 @@
         <v>0.882000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -805,4 +1880,171 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C650FE1-F1C5-40B6-A628-C7693AE9A8DC}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-30</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <f>180/3.142*ATAN2(B2,C2)</f>
+        <v>51.333535717008886</v>
+      </c>
+      <c r="E2">
+        <v>51.058</v>
+      </c>
+      <c r="F2" s="1">
+        <f>ABS(E2-D2)</f>
+        <v>0.27553571700888568</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-25</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D10" si="0">180/3.142*ATAN2(B3,C3)</f>
+        <v>51.333535717008886</v>
+      </c>
+      <c r="E3">
+        <v>51.052999999999997</v>
+      </c>
+      <c r="F3" s="1">
+        <f>ABS(E3-D3)</f>
+        <v>0.28053571700888824</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-20</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>51.333535717008886</v>
+      </c>
+      <c r="E4">
+        <v>51.058999999999997</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F6" si="1">ABS(E4-D4)</f>
+        <v>0.27453571700888801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-15</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>51.333535717008886</v>
+      </c>
+      <c r="E5">
+        <v>51.057000000000002</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.27653571700888335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-10</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>51.333535717008886</v>
+      </c>
+      <c r="E6">
+        <v>51.055999999999997</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.27753571700888813</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>